<commit_message>
add limit logic transition hints for startup procedure
</commit_message>
<xml_diff>
--- a/docs/design/pss/control-logic/limit-logic/truth-table-mode-set-reset.xlsx
+++ b/docs/design/pss/control-logic/limit-logic/truth-table-mode-set-reset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\240613_HFU_SMA_Master_Thesis\obat\docs\design\pss\control-logic\limit-logic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690AA5C7-CB6D-47E0-BB7C-1909FCF62EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30F9C87-50AD-48D1-98EA-2D17250029B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC98877B-7BEB-4BB2-B5C5-766C6DD71E55}"/>
   </bookViews>
@@ -62,9 +62,10 @@
           </rPr>
           <t xml:space="preserve">
 Pascal_Guttmann:
-Gapping Switching is implemented via RS Latches.
+Gapping Switching is implemented via RS Latches. (Set only, when no Mode is active)
 A Transition is possible from the resetted mode "MODE R" to the set mode "MODE S".
-For robustness, if no MODE is active VC can be set.</t>
+At startup: RC timer, Reset/not enable
+start timer, when no config error CNF_ERROR = !AND(XOR(REF==U, REF==I), LCL&lt;UCL, LVL&lt;UVL)</t>
         </r>
       </text>
     </comment>
@@ -313,11 +314,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -350,22 +348,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF3F3F3F"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF3F3F3F"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -423,6 +426,9 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="double">
           <color indexed="64"/>
@@ -430,46 +436,17 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF3F3F3F"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF3F3F3F"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -484,27 +461,23 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA27195F-AE67-4F40-BF86-8BB43EC4ABE0}" name="Table1" displayName="Table1" ref="A1:N15" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="15" headerRowCellStyle="Output" dataCellStyle="Output">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA27195F-AE67-4F40-BF86-8BB43EC4ABE0}" name="Table1" displayName="Table1" ref="A1:N15" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" headerRowCellStyle="Output" dataCellStyle="Output">
   <autoFilter ref="A1:N15" xr:uid="{DA27195F-AE67-4F40-BF86-8BB43EC4ABE0}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{1D4D7CFA-EEFF-49CC-B6E3-CD37603DD213}" name="REF" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{E872F240-7070-487A-A7D1-E1B89183F30B}" name="LVLE" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{9AA69D7A-5BF5-44B1-ABD4-05066FAE69F1}" name="UVLE" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{D35A1935-5AEF-4597-AAF2-4FABFEE34F68}" name="LCLE" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{F1D526A6-C7EC-4884-86E9-64A0A4604C76}" name="UCLE" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{D0B5C53A-88DE-4A9E-976F-E36A9D1BA20B}" name="MSTT" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{E8A2B42D-CA06-4DC8-83BA-A70DFD2D6854}" name="MGTT" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{B2368061-9F18-4098-9A4F-4B06E760DF3C}" name="VC" dataDxfId="7" dataCellStyle="Output"/>
-    <tableColumn id="9" xr3:uid="{D8248A7F-5964-4738-95C1-27D91A1C0045}" name="LCLC" dataDxfId="6" dataCellStyle="Output"/>
-    <tableColumn id="10" xr3:uid="{0434A4F2-0D31-487B-8538-80040501D86F}" name="UCLC" dataDxfId="5" dataCellStyle="Output"/>
-    <tableColumn id="11" xr3:uid="{5AC7D3EE-81C7-4EBC-9BD0-7AE42A9E9FDC}" name="CC" dataDxfId="4" dataCellStyle="Output"/>
-    <tableColumn id="12" xr3:uid="{CF1A8950-CF2C-496F-A1FD-F8F7FAF8BC53}" name="LVLC" dataDxfId="3" dataCellStyle="Output"/>
-    <tableColumn id="13" xr3:uid="{AC990C43-4F8C-41A5-A109-40604E315B53}" name="UVLC" dataDxfId="2" dataCellStyle="Output"/>
+    <tableColumn id="1" xr3:uid="{1D4D7CFA-EEFF-49CC-B6E3-CD37603DD213}" name="REF" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{E872F240-7070-487A-A7D1-E1B89183F30B}" name="LVLE" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{9AA69D7A-5BF5-44B1-ABD4-05066FAE69F1}" name="UVLE" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{D35A1935-5AEF-4597-AAF2-4FABFEE34F68}" name="LCLE" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{F1D526A6-C7EC-4884-86E9-64A0A4604C76}" name="UCLE" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{D0B5C53A-88DE-4A9E-976F-E36A9D1BA20B}" name="MSTT" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{E8A2B42D-CA06-4DC8-83BA-A70DFD2D6854}" name="MGTT" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{B2368061-9F18-4098-9A4F-4B06E760DF3C}" name="VC" dataDxfId="8" dataCellStyle="Output"/>
+    <tableColumn id="9" xr3:uid="{D8248A7F-5964-4738-95C1-27D91A1C0045}" name="LCLC" dataDxfId="7" dataCellStyle="Output"/>
+    <tableColumn id="10" xr3:uid="{0434A4F2-0D31-487B-8538-80040501D86F}" name="UCLC" dataDxfId="6" dataCellStyle="Output"/>
+    <tableColumn id="11" xr3:uid="{5AC7D3EE-81C7-4EBC-9BD0-7AE42A9E9FDC}" name="CC" dataDxfId="5" dataCellStyle="Output"/>
+    <tableColumn id="12" xr3:uid="{CF1A8950-CF2C-496F-A1FD-F8F7FAF8BC53}" name="LVLC" dataDxfId="4" dataCellStyle="Output"/>
+    <tableColumn id="13" xr3:uid="{AC990C43-4F8C-41A5-A109-40604E315B53}" name="UVLC" dataDxfId="3" dataCellStyle="Output"/>
     <tableColumn id="14" xr3:uid="{8E911C9F-856A-4EA8-8118-CAA6EB0E94CF}" name="Excl. By Design"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -837,63 +810,63 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="7" style="3" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="7" style="2" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" style="2" customWidth="1"/>
     <col min="14" max="14" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="8" t="s">
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -901,153 +874,153 @@
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="6" t="s">
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" s="3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" s="3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="3" t="s">
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N5" t="s">
@@ -1055,92 +1028,92 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="3" t="s">
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="3" t="s">
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="N8" t="s">
@@ -1148,154 +1121,154 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="3" t="s">
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M10" s="3" t="s">
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="2">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="3" t="s">
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M12" s="3" t="s">
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N12" t="s">
@@ -1303,92 +1276,92 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M13" s="3" t="s">
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L14" s="3" t="s">
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M15" s="3" t="s">
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="N15" t="s">
@@ -1397,14 +1370,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
-      <formula>1</formula>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
-      <formula>"S"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix limit-logic state transition from U to I Mode
</commit_message>
<xml_diff>
--- a/docs/design/pss/control-logic/limit-logic/truth-table-mode-set-reset.xlsx
+++ b/docs/design/pss/control-logic/limit-logic/truth-table-mode-set-reset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\240613_HFU_SMA_Master_Thesis\obat\docs\design\pss\control-logic\limit-logic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30F9C87-50AD-48D1-98EA-2D17250029B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A18A924-7554-4F34-A0C7-61062448FB2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CC98877B-7BEB-4BB2-B5C5-766C6DD71E55}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="19">
   <si>
     <t>LCLE</t>
   </si>
@@ -163,7 +163,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +192,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -314,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -323,12 +330,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -343,51 +344,146 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF3F3F3F"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF3F3F3F"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF3F3F3F"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF3F3F3F"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF3F3F3F"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF3F3F3F"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thick">
           <color rgb="FF3F3F3F"/>
         </left>
@@ -400,9 +496,28 @@
         <bottom style="thin">
           <color rgb="FF3F3F3F"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -462,23 +577,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA27195F-AE67-4F40-BF86-8BB43EC4ABE0}" name="Table1" displayName="Table1" ref="A1:N15" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" headerRowCellStyle="Output" dataCellStyle="Output">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA27195F-AE67-4F40-BF86-8BB43EC4ABE0}" name="Table1" displayName="Table1" ref="A1:N15" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" headerRowCellStyle="Output" dataCellStyle="Output">
   <autoFilter ref="A1:N15" xr:uid="{DA27195F-AE67-4F40-BF86-8BB43EC4ABE0}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{1D4D7CFA-EEFF-49CC-B6E3-CD37603DD213}" name="REF" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{E872F240-7070-487A-A7D1-E1B89183F30B}" name="LVLE" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{9AA69D7A-5BF5-44B1-ABD4-05066FAE69F1}" name="UVLE" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{D35A1935-5AEF-4597-AAF2-4FABFEE34F68}" name="LCLE" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{F1D526A6-C7EC-4884-86E9-64A0A4604C76}" name="UCLE" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{D0B5C53A-88DE-4A9E-976F-E36A9D1BA20B}" name="MSTT" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{E8A2B42D-CA06-4DC8-83BA-A70DFD2D6854}" name="MGTT" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{B2368061-9F18-4098-9A4F-4B06E760DF3C}" name="VC" dataDxfId="8" dataCellStyle="Output"/>
-    <tableColumn id="9" xr3:uid="{D8248A7F-5964-4738-95C1-27D91A1C0045}" name="LCLC" dataDxfId="7" dataCellStyle="Output"/>
-    <tableColumn id="10" xr3:uid="{0434A4F2-0D31-487B-8538-80040501D86F}" name="UCLC" dataDxfId="6" dataCellStyle="Output"/>
-    <tableColumn id="11" xr3:uid="{5AC7D3EE-81C7-4EBC-9BD0-7AE42A9E9FDC}" name="CC" dataDxfId="5" dataCellStyle="Output"/>
-    <tableColumn id="12" xr3:uid="{CF1A8950-CF2C-496F-A1FD-F8F7FAF8BC53}" name="LVLC" dataDxfId="4" dataCellStyle="Output"/>
-    <tableColumn id="13" xr3:uid="{AC990C43-4F8C-41A5-A109-40604E315B53}" name="UVLC" dataDxfId="3" dataCellStyle="Output"/>
-    <tableColumn id="14" xr3:uid="{8E911C9F-856A-4EA8-8118-CAA6EB0E94CF}" name="Excl. By Design"/>
+    <tableColumn id="1" xr3:uid="{1D4D7CFA-EEFF-49CC-B6E3-CD37603DD213}" name="REF" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{E872F240-7070-487A-A7D1-E1B89183F30B}" name="LVLE" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{9AA69D7A-5BF5-44B1-ABD4-05066FAE69F1}" name="UVLE" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{D35A1935-5AEF-4597-AAF2-4FABFEE34F68}" name="LCLE" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{F1D526A6-C7EC-4884-86E9-64A0A4604C76}" name="UCLE" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{D0B5C53A-88DE-4A9E-976F-E36A9D1BA20B}" name="MSTT" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{E8A2B42D-CA06-4DC8-83BA-A70DFD2D6854}" name="MGTT" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{B2368061-9F18-4098-9A4F-4B06E760DF3C}" name="VC" dataDxfId="6" dataCellStyle="Output"/>
+    <tableColumn id="9" xr3:uid="{D8248A7F-5964-4738-95C1-27D91A1C0045}" name="LCLC" dataDxfId="5" dataCellStyle="Output"/>
+    <tableColumn id="10" xr3:uid="{0434A4F2-0D31-487B-8538-80040501D86F}" name="UCLC" dataDxfId="4" dataCellStyle="Output"/>
+    <tableColumn id="11" xr3:uid="{5AC7D3EE-81C7-4EBC-9BD0-7AE42A9E9FDC}" name="CC" dataDxfId="3" dataCellStyle="Output"/>
+    <tableColumn id="12" xr3:uid="{CF1A8950-CF2C-496F-A1FD-F8F7FAF8BC53}" name="LVLC" dataDxfId="2" dataCellStyle="Output"/>
+    <tableColumn id="13" xr3:uid="{AC990C43-4F8C-41A5-A109-40604E315B53}" name="UVLC" dataDxfId="0" dataCellStyle="Output"/>
+    <tableColumn id="14" xr3:uid="{8E911C9F-856A-4EA8-8118-CAA6EB0E94CF}" name="Excl. By Design" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -805,7 +920,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q14" sqref="Q14"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,56 +932,52 @@
     <col min="5" max="5" width="6.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="6.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="7" style="2" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="3" customWidth="1"/>
+    <col min="9" max="13" width="6.7109375" style="2" customWidth="1"/>
     <col min="14" max="14" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="D1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -892,18 +1003,18 @@
       <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="5" t="s">
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="11" t="s">
         <v>18</v>
       </c>
     </row>
@@ -929,19 +1040,20 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" s="2" t="s">
+      <c r="I3" s="8"/>
+      <c r="J3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -967,19 +1079,20 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" s="2" t="s">
+      <c r="I4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1005,22 +1118,22 @@
       <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="2" t="s">
+      <c r="I5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="8" t="s">
         <v>18</v>
       </c>
       <c r="N5" t="s">
@@ -1049,11 +1162,21 @@
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="2" t="s">
+      <c r="H6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8" t="s">
         <v>17</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1078,11 +1201,21 @@
       <c r="G7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="2" t="s">
+      <c r="H7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>17</v>
+      </c>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1107,14 +1240,23 @@
       <c r="G8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="2" t="s">
+      <c r="H8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="8" t="s">
         <v>17</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="N8" t="s">
         <v>5</v>
@@ -1142,18 +1284,20 @@
       <c r="G9" s="1">
         <v>0</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="2" t="s">
+      <c r="H9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1177,19 +1321,20 @@
       <c r="G10" s="1">
         <v>1</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="2" t="s">
+      <c r="H10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="L10" s="8"/>
+      <c r="M10" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1215,21 +1360,22 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11" s="2" t="s">
+      <c r="H11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="L11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1253,22 +1399,22 @@
       <c r="G12" s="1">
         <v>1</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" s="2" t="s">
+      <c r="H12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M12" s="2" t="s">
+      <c r="L12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" s="8" t="s">
         <v>18</v>
       </c>
       <c r="N12" t="s">
@@ -1297,10 +1443,20 @@
       <c r="G13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M13" s="2" t="s">
+      <c r="H13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1326,12 +1482,22 @@
       <c r="G14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L14" s="2" t="s">
+      <c r="H14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" s="8" t="s">
         <v>17</v>
       </c>
+      <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1355,13 +1521,22 @@
       <c r="G15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L15" s="2" t="s">
+      <c r="H15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="M15" s="8" t="s">
         <v>17</v>
       </c>
       <c r="N15" t="s">
@@ -1370,13 +1545,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>